<commit_message>
AOR1 K2 druga tabela je gotova
</commit_message>
<xml_diff>
--- a/pythonProject/Test.xlsx
+++ b/pythonProject/Test.xlsx
@@ -14,39 +14,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Виртуелна адреса</t>
-  </si>
-  <si>
-    <t>Тип</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Segment</t>
-  </si>
-  <si>
-    <t>Page</t>
-  </si>
-  <si>
-    <t>Word</t>
-  </si>
-  <si>
-    <t>Tag</t>
-  </si>
-  <si>
-    <t>Entry</t>
-  </si>
-  <si>
-    <t>Коментар</t>
-  </si>
-  <si>
-    <t>Block</t>
-  </si>
-  <si>
-    <t>Физичка адреса</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Адресе у меморији са којих је учитана инструкција</t>
+  </si>
+  <si>
+    <t>IR31..24</t>
+  </si>
+  <si>
+    <t>IR23..16</t>
+  </si>
+  <si>
+    <t>IR15..8</t>
+  </si>
+  <si>
+    <t>IR7..0</t>
+  </si>
+  <si>
+    <t>Инструкција</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Адресе у меморији са којих је учитана адреса операнда</t>
+  </si>
+  <si>
+    <t>Адресе у меморији са којих је учитан операнд</t>
+  </si>
+  <si>
+    <t>Операнд</t>
+  </si>
+  <si>
+    <t>Нови садржај регистара опште намене</t>
+  </si>
+  <si>
+    <t>Меморијске адресе којима се приступа у овој фази</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Акумулатор</t>
+  </si>
+  <si>
+    <t>Нови садржај регистара и меморијских локација који су промењени у овој фази</t>
   </si>
 </sst>
 </file>
@@ -434,13 +458,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:8" ht="40" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,17 +494,100 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="12" spans="1:8" ht="40" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="23" spans="1:10" ht="40" customHeight="1">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H23:J23"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A13:H19">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24:J30">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A2:H8">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
       <formula>0</formula>

</xml_diff>